<commit_message>
env can run now, but some parameter need to be modified by model browser
</commit_message>
<xml_diff>
--- a/config/cfg_crlc/profile_df_1580.xlsx
+++ b/config/cfg_crlc/profile_df_1580.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digestion\tiny_ssu_calc\cfg_crlc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digestion\tiny_ssu_calc\config\cfg_crlc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,11 +34,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cvc1</t>
+    <t>parab</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>parab</t>
+    <t>cvc4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -373,7 +373,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -391,7 +391,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -402,7 +402,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -413,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -424,7 +424,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -435,7 +435,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>-0.36</v>
@@ -457,7 +457,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>-0.36</v>

</xml_diff>